<commit_message>
python-National Day For Travel Without So Many People！I run~
Signed-off-by: chenyabin1 <“chenyabin@jd.com”>
</commit_message>
<xml_diff>
--- a/edition_sample/NationalDayTravel/qunar_place.xlsx
+++ b/edition_sample/NationalDayTravel/qunar_place.xlsx
@@ -532,50 +532,50 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>528078619</v>
+        <v>1514814960</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>大报恩寺遗址公园</t>
+          <t>中山陵</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>无</t>
+          <t>5A</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E5" t="n">
-        <v>39.5</v>
+        <v>25.1</v>
       </c>
       <c r="F5" t="n">
-        <v>1514</v>
+        <v>1918</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>江苏·南京·秦淮区</t>
+          <t>江苏·南京·钟山风景区</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>118.787634,32.015811</t>
+          <t>118.860335,32.063934</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>长干里是江南佛教圣地素有“佛陀里”之美</t>
+          <t>建筑名家之杰作，有着极高的艺术价值</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>1514814960</v>
+        <v>3319594683</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>中山陵</t>
+          <t>趵突泉公园</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -584,37 +584,37 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>5</v>
+        <v>4.7</v>
       </c>
       <c r="E6" t="n">
-        <v>25.1</v>
+        <v>20</v>
       </c>
       <c r="F6" t="n">
-        <v>1918</v>
+        <v>2021</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>江苏·南京·钟山风景区</t>
+          <t>山东·济南·天下第一泉风景区</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>118.860335,32.063934</t>
+          <t>117.02264,36.667808</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>建筑名家之杰作，有着极高的艺术价值</t>
+          <t>康熙皇帝赞誉的天下名泉</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>3319594683</v>
+        <v>2778205010</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>趵突泉公园</t>
+          <t>夫子庙</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -623,91 +623,91 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>4.7</v>
+        <v>4.4</v>
       </c>
       <c r="E7" t="n">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F7" t="n">
-        <v>2021</v>
+        <v>1118</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>山东·济南·天下第一泉风景区</t>
+          <t>江苏·南京·秦淮区</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>117.02264,36.667808</t>
+          <t>118.795398,32.026977</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>康熙皇帝赞誉的天下名泉</t>
+          <t>一条长江路，半部民国史</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>1040506812</v>
+        <v>1311542410</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>银杏湖乐园</t>
+          <t>临潼博物馆</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>无</t>
+          <t>3A</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="E8" t="n">
-        <v>205.7</v>
+        <v>128</v>
       </c>
       <c r="F8" t="n">
-        <v>626</v>
+        <v>2451</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>江苏·南京·江宁区</t>
+          <t>陕西·西安·临潼区</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>118.721425,31.811687</t>
+          <t>109.223096,34.370575</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>让小朋友能够体验互动的快乐</t>
+          <t>珍藏有西周青铜器、唯一记载武王伐纣的遗物</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>2778205010</v>
+        <v>528078619</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>夫子庙</t>
+          <t>大报恩寺遗址公园</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>5A</t>
+          <t>无</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>4.4</v>
+        <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>24</v>
+        <v>39.5</v>
       </c>
       <c r="F9" t="n">
-        <v>1118</v>
+        <v>1514</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -716,61 +716,61 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>118.795398,32.026977</t>
+          <t>118.787634,32.015811</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>一条长江路，半部民国史</t>
+          <t>长干里是江南佛教圣地素有“佛陀里”之美</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>1311542410</v>
+        <v>3604815083</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>临潼博物馆</t>
+          <t>泉城广场</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>3A</t>
+          <t>无</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>3.5</v>
+        <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>128</v>
+        <v>28</v>
       </c>
       <c r="F10" t="n">
-        <v>2451</v>
+        <v>58</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>陕西·西安·临潼区</t>
+          <t>山东·济南·历下区</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>109.223096,34.370575</t>
+          <t>117.028281,36.667555</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>珍藏有西周青铜器、唯一记载武王伐纣的遗物</t>
+          <t>市民休憩盘桓之胜地</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>837643663</v>
+        <v>274697750</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>柳州卡乐星球</t>
+          <t>洞天仙境</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -782,151 +782,151 @@
         <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="F11" t="n">
-        <v>558</v>
+        <v>3099</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>广西·柳州</t>
+          <t>广东·清远·英西峰林</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>109.553059,24.392098</t>
+          <t>112.906583,24.158095</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>“科技版欢乐谷”，育智于乐</t>
+          <t>在九龙，观洞天仙境，九龙在渊，福地洞天</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>3604815083</v>
+        <v>3787214683</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>泉城广场</t>
+          <t>兴隆山</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>无</t>
+          <t>4A</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0</v>
+        <v>3.6</v>
       </c>
       <c r="E12" t="n">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="F12" t="n">
-        <v>58</v>
+        <v>230</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>山东·济南·历下区</t>
+          <t>甘肃·兰州·榆中县</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>117.028281,36.667555</t>
+          <t>104.123459,35.832808</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>市民休憩盘桓之胜地</t>
+          <t>奇峰叠翠、飞泉流湍、森林苍郁、风景旖旎</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>274697750</v>
+        <v>1537503131</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>洞天仙境</t>
+          <t>独秀峰王城景区</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>无</t>
+          <t>5A</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>0</v>
+        <v>3.6</v>
       </c>
       <c r="E13" t="n">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="F13" t="n">
-        <v>3099</v>
+        <v>820</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>广东·清远·英西峰林</t>
+          <t>广西·桂林·秀峰区</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>112.906583,24.158095</t>
+          <t>110.305678,25.289462</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>在九龙，观洞天仙境，九龙在渊，福地洞天</t>
+          <t>明代王府清朝贡院所在地，阅尽王城知桂林</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>782127360</v>
+        <v>3907699975</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>广州二龙山花园</t>
+          <t>槟榔谷黎苗文化区</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>无</t>
+          <t>5A</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>0</v>
+        <v>3.6</v>
       </c>
       <c r="E14" t="n">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="F14" t="n">
-        <v>54</v>
+        <v>738</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>广东·广州·增城</t>
+          <t>海南·保亭</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>113.744701,23.361559</t>
+          <t>109.677278,18.466556</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>中国美景与欧美小镇风情相结合的度假胜地</t>
+          <t>一个逃逸世俗的心灵驿站</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>3787214683</v>
+        <v>290674956</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>兴隆山</t>
+          <t>大明湖</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -935,115 +935,115 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>3.6</v>
+        <v>5</v>
       </c>
       <c r="E15" t="n">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="F15" t="n">
-        <v>230</v>
+        <v>110</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>甘肃·兰州·榆中县</t>
+          <t>山东·济南·历下区</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>104.123459,35.832808</t>
+          <t>117.029659,36.679466</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>奇峰叠翠、飞泉流湍、森林苍郁、风景旖旎</t>
+          <t>皇上，你还记得大明湖畔的夏雨荷吗</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>1537503131</v>
+        <v>837719622</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>独秀峰王城景区</t>
+          <t>厦门湾·白塘湾火山公园</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>5A</t>
+          <t>无</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>3.6</v>
+        <v>0</v>
       </c>
       <c r="E16" t="n">
-        <v>79</v>
+        <v>43</v>
       </c>
       <c r="F16" t="n">
-        <v>820</v>
+        <v>304</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>广西·桂林·秀峰区</t>
+          <t>福建·漳州·龙海市</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>110.305678,25.289462</t>
+          <t>118.053033,24.231948</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>明代王府清朝贡院所在地，阅尽王城知桂林</t>
+          <t>2460万年前海底兵马俑</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>3907699975</v>
+        <v>4131159698</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>槟榔谷黎苗文化区</t>
+          <t>天津之眼摩天轮</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>5A</t>
+          <t>4A</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>3.6</v>
+        <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>35</v>
+        <v>1.4</v>
       </c>
       <c r="F17" t="n">
-        <v>738</v>
+        <v>120</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>海南·保亭</t>
+          <t>天津·天津·河北区</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>109.677278,18.466556</t>
+          <t>117.193805,39.160233</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>一个逃逸世俗的心灵驿站</t>
+          <t>建在桥上的摩天轮</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>290674956</v>
+        <v>290526810</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>大明湖</t>
+          <t>南京大屠杀遇难同胞纪念馆</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1052,76 +1052,76 @@
         </is>
       </c>
       <c r="D18" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="E18" t="n">
         <v>5</v>
       </c>
-      <c r="E18" t="n">
-        <v>28</v>
-      </c>
       <c r="F18" t="n">
-        <v>110</v>
+        <v>158</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>山东·济南·历下区</t>
+          <t>江苏·南京·建邺区</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>117.029659,36.679466</t>
+          <t>118.748954,32.040883</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>皇上，你还记得大明湖畔的夏雨荷吗</t>
+          <t>寸草不生，几棵枯树仕立，气氛凄凉</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>837719622</v>
+        <v>65647061</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>厦门湾·白塘湾火山公园</t>
+          <t>南京阅江楼</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>无</t>
+          <t>4A</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>0</v>
+        <v>3.9</v>
       </c>
       <c r="E19" t="n">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="F19" t="n">
-        <v>304</v>
+        <v>562</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>福建·漳州·龙海市</t>
+          <t>江苏·南京·下关区</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>118.053033,24.231948</t>
+          <t>118.75312,32.099764</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>2460万年前海底兵马俑</t>
+          <t>狮子山巅凭栏阅江，品六百年传奇之楼</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>2225247801</v>
+        <v>1397926396</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>世贸宽厚里</t>
+          <t>秦始皇陵丽山园景区</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1133,112 +1133,112 @@
         <v>0</v>
       </c>
       <c r="E20" t="n">
-        <v>98</v>
+        <v>1.6</v>
       </c>
       <c r="F20" t="n">
-        <v>22</v>
+        <v>314</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>山东·济南·历下区</t>
+          <t>陕西·西安·秦始皇陵博物院（兵马俑）</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>117.038713,36.670288</t>
+          <t>109.265495,34.385836</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>一处新的济南老街巷</t>
+          <t>秦始皇帝陵博物院的组成部分</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>4131159698</v>
+        <v>4050084688</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>天津之眼摩天轮</t>
+          <t>熊牧场</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>4A</t>
+          <t>无</t>
         </is>
       </c>
       <c r="D21" t="n">
         <v>0</v>
       </c>
       <c r="E21" t="n">
-        <v>1.4</v>
+        <v>56</v>
       </c>
       <c r="F21" t="n">
-        <v>120</v>
+        <v>86</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>天津·天津·河北区</t>
+          <t>山东·青岛·崂山区</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>117.193805,39.160233</t>
+          <t>120.517176,36.101748</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>建在桥上的摩天轮</t>
+          <t>来熊牧场近距离接触各种熊</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>290526810</v>
+        <v>837643663</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>南京大屠杀遇难同胞纪念馆</t>
+          <t>柳州卡乐星球</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>4A</t>
+          <t>无</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>3.8</v>
+        <v>0</v>
       </c>
       <c r="E22" t="n">
-        <v>5</v>
+        <v>59</v>
       </c>
       <c r="F22" t="n">
-        <v>158</v>
+        <v>558</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>江苏·南京·建邺区</t>
+          <t>广西·柳州</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>118.748954,32.040883</t>
+          <t>109.553059,24.392098</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>寸草不生，几棵枯树仕立，气氛凄凉</t>
+          <t>“科技版欢乐谷”，育智于乐</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>2648582804</v>
+        <v>3497524618</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Boom Park动物主题公园</t>
+          <t>大沽口炮台遗址</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1247,76 +1247,76 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>0</v>
+        <v>3.7</v>
       </c>
       <c r="E23" t="n">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="F23" t="n">
-        <v>8</v>
+        <v>86</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>四川·绵阳</t>
+          <t>天津·天津·滨海新区</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>104.656896,31.465894</t>
+          <t>117.716282,38.983338</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>适合全民游玩的都市大型室内动物主题公园</t>
+          <t>首都的海上门户，近代海防遗址之一</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>65647061</v>
+        <v>1561296550</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>南京阅江楼</t>
+          <t>诚毅科技探索中心</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>4A</t>
+          <t>无</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>3.9</v>
+        <v>0</v>
       </c>
       <c r="E24" t="n">
-        <v>28</v>
+        <v>58.9</v>
       </c>
       <c r="F24" t="n">
-        <v>562</v>
+        <v>230</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>江苏·南京·下关区</t>
+          <t>福建·厦门·集美区</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>118.75312,32.099764</t>
+          <t>118.064062,24.598948</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>狮子山巅凭栏阅江，品六百年传奇之楼</t>
+          <t>全国首家以探索为主题的大型科普乐园</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>1397926396</v>
+        <v>2615113548</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>秦始皇陵丽山园景区</t>
+          <t>意式风情街</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1328,34 +1328,34 @@
         <v>0</v>
       </c>
       <c r="E25" t="n">
-        <v>1.6</v>
+        <v>75</v>
       </c>
       <c r="F25" t="n">
-        <v>314</v>
+        <v>90</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>陕西·西安·秦始皇陵博物院（兵马俑）</t>
+          <t>天津·天津·河北区</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>109.265495,34.385836</t>
+          <t>117.206871,39.140884</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>秦始皇帝陵博物院的组成部分</t>
+          <t>浓浓意大利风情，让你不出国游遍意大利</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>4050084688</v>
+        <v>782127360</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>熊牧场</t>
+          <t>广州二龙山花园</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1367,34 +1367,34 @@
         <v>0</v>
       </c>
       <c r="E26" t="n">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="F26" t="n">
-        <v>86</v>
+        <v>54</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>山东·青岛·崂山区</t>
+          <t>广东·广州·增城</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>120.517176,36.101748</t>
+          <t>113.744701,23.361559</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>来熊牧场近距离接触各种熊</t>
+          <t>中国美景与欧美小镇风情相结合的度假胜地</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>3497524618</v>
+        <v>2971839392</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>大沽口炮台遗址</t>
+          <t>瓷房子</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1403,37 +1403,37 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>3.7</v>
+        <v>4.1</v>
       </c>
       <c r="E27" t="n">
-        <v>10</v>
+        <v>0.5</v>
       </c>
       <c r="F27" t="n">
-        <v>86</v>
+        <v>186</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>天津·天津·滨海新区</t>
+          <t>天津·天津·和平区</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>117.716282,38.983338</t>
+          <t>117.202575,39.124825</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>首都的海上门户，近代海防遗址之一</t>
+          <t>中国古典艺术品与西洋建筑的完美结合</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>1561296550</v>
+        <v>3485756374</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>诚毅科技探索中心</t>
+          <t>红珠山森林温泉</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1445,34 +1445,34 @@
         <v>0</v>
       </c>
       <c r="E28" t="n">
-        <v>58.9</v>
+        <v>138</v>
       </c>
       <c r="F28" t="n">
-        <v>230</v>
+        <v>92</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>福建·厦门·集美区</t>
+          <t>四川·乐山·峨眉山市</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>118.064062,24.598948</t>
+          <t>103.449416,29.569811</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>全国首家以探索为主题的大型科普乐园</t>
+          <t>树林之间点缀的19个温泉池极具特色</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>2615113548</v>
+        <v>2088463447</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>意式风情街</t>
+          <t>悉尼水族馆</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1481,37 +1481,37 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>0</v>
+        <v>3.6</v>
       </c>
       <c r="E29" t="n">
-        <v>75</v>
+        <v>110</v>
       </c>
       <c r="F29" t="n">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>天津·天津·河北区</t>
+          <t>新南威尔士州·悉尼</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>117.206871,39.140884</t>
+          <t>151.202211035276,-33.8700138</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>浓浓意大利风情，让你不出国游遍意大利</t>
+          <t>在密闭的透明容器里与斑斓的热带鱼共舞</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>2971839392</v>
+        <v>2225247801</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>瓷房子</t>
+          <t>世贸宽厚里</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1520,37 +1520,37 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>4.1</v>
+        <v>0</v>
       </c>
       <c r="E30" t="n">
-        <v>0.5</v>
+        <v>98</v>
       </c>
       <c r="F30" t="n">
-        <v>186</v>
+        <v>22</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>天津·天津·和平区</t>
+          <t>山东·济南·历下区</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>117.202575,39.124825</t>
+          <t>117.038713,36.670288</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>中国古典艺术品与西洋建筑的完美结合</t>
+          <t>一处新的济南老街巷</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>3485756374</v>
+        <v>2648582804</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>红珠山森林温泉</t>
+          <t>Boom Park动物主题公园</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1562,34 +1562,34 @@
         <v>0</v>
       </c>
       <c r="E31" t="n">
-        <v>138</v>
+        <v>18</v>
       </c>
       <c r="F31" t="n">
-        <v>92</v>
+        <v>8</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>四川·乐山·峨眉山市</t>
+          <t>四川·绵阳</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>103.449416,29.569811</t>
+          <t>104.656896,31.465894</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>树林之间点缀的19个温泉池极具特色</t>
+          <t>适合全民游玩的都市大型室内动物主题公园</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>2088463447</v>
+        <v>2731148767</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>悉尼水族馆</t>
+          <t>宁乡灰汤紫龙湾温泉度假区</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1598,37 +1598,37 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>3.6</v>
+        <v>3.5</v>
       </c>
       <c r="E32" t="n">
-        <v>110</v>
+        <v>166</v>
       </c>
       <c r="F32" t="n">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>新南威尔士州·悉尼</t>
+          <t>湖南·长沙·宁乡县</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>151.202211035276,-33.8700138</t>
+          <t>112.351923,27.985351</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>在密闭的透明容器里与斑斓的热带鱼共舞</t>
+          <t>水质晶莹如玉，沸如滚汤，保健功效显著</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>2731148767</v>
+        <v>1966972638</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>宁乡灰汤紫龙湾温泉度假区</t>
+          <t>伊酷拉探索岛</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1637,115 +1637,115 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>3.5</v>
+        <v>0</v>
       </c>
       <c r="E33" t="n">
-        <v>166</v>
+        <v>55</v>
       </c>
       <c r="F33" t="n">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>湖南·长沙·宁乡县</t>
+          <t>江苏·常州·天宁区</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>112.351923,27.985351</t>
+          <t>120.143815,31.84411</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>水质晶莹如玉，沸如滚汤，保健功效显著</t>
+          <t>位于常州天宁区牟家村，占地面积约100亩，响应美丽乡村建设的号召，顺应国内儿童亲子市场发展趋势，充分结合常州市天宁区的特</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>1966972638</v>
+        <v>1811187320</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>伊酷拉探索岛</t>
+          <t>千佛山景区</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>无</t>
+          <t>4A</t>
         </is>
       </c>
       <c r="D34" t="n">
         <v>0</v>
       </c>
       <c r="E34" t="n">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="F34" t="n">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>江苏·常州·天宁区</t>
+          <t>浙江·丽水·遂昌县</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>120.143815,31.84411</t>
+          <t>119.034089,28.479885</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>位于常州天宁区牟家村，占地面积约100亩，响应美丽乡村建设的号召，顺应国内儿童亲子市场发展趋势，充分结合常州市天宁区的特</t>
+          <t>江南小九寨</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>1811187320</v>
+        <v>730535106</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>千佛山景区</t>
+          <t>悉尼港</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>4A</t>
+          <t>无</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>0</v>
+        <v>3.6</v>
       </c>
       <c r="E35" t="n">
-        <v>63</v>
+        <v>218</v>
       </c>
       <c r="F35" t="n">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>浙江·丽水·遂昌县</t>
+          <t>新南威尔士州·悉尼</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>119.034089,28.479885</t>
+          <t>151.241928,-33.857506</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>江南小九寨</t>
+          <t>悉尼的天然海港，这里的落日让人难以忘怀</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>25603024</v>
+        <v>3210601919</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>长江观音景区</t>
+          <t>古文化街码头</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1757,34 +1757,34 @@
         <v>0</v>
       </c>
       <c r="E36" t="n">
-        <v>21.5</v>
+        <v>64</v>
       </c>
       <c r="F36" t="n">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>江苏·南京·栖霞区</t>
+          <t>天津·天津·南开区</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>118.803931,32.133416</t>
+          <t>117.201171,39.15063</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>长江沿岸以观音文化为主题的景区</t>
+          <t>古文化街的入口之一</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>2608360544</v>
+        <v>2935695043</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>悉尼杜莎夫人蜡像馆</t>
+          <t>黑虎泉</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1793,76 +1793,76 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>0</v>
+        <v>3.9</v>
       </c>
       <c r="E37" t="n">
-        <v>110</v>
+        <v>6</v>
       </c>
       <c r="F37" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>新南威尔士州·悉尼</t>
+          <t>山东·济南·历下区</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>151.201508,-33.869791</t>
+          <t>117.039676,36.668445</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>看美丽栩栩如生的澳洲名模、皮特夫妇等</t>
+          <t>石雕虎头泉水喷出，波澜汹汹，水声喧喧</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>730535106</v>
+        <v>1192886682</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>悉尼港</t>
+          <t>花水湾温泉旅游度假区</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>无</t>
+          <t>4A</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>3.6</v>
+        <v>3.5</v>
       </c>
       <c r="E38" t="n">
-        <v>218</v>
+        <v>47</v>
       </c>
       <c r="F38" t="n">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>新南威尔士州·悉尼</t>
+          <t>四川·成都·大邑县</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>151.241928,-33.857506</t>
+          <t>103.268238,30.569815</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>悉尼的天然海港，这里的落日让人难以忘怀</t>
+          <t>环境优美，休闲度假的好去处</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>3210601919</v>
+        <v>2437128342</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>古文化街码头</t>
+          <t>海河公园</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1877,31 +1877,31 @@
         <v>64</v>
       </c>
       <c r="F39" t="n">
-        <v>62</v>
+        <v>40</v>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>天津·天津·南开区</t>
+          <t>天津·天津·和平区</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>117.201171,39.15063</t>
+          <t>117.218779,39.136942</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>古文化街的入口之一</t>
+          <t>海河公园、游玩、休憩的地方之一。在三岔口紧靠狮子林桥的水面上，有两组铜质塑像，这是海河公园的起点。其中，一组塑像是两条雄</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>4263621879</v>
+        <v>2983420679</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>香道温泉会馆</t>
+          <t>大堡礁</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1913,34 +1913,34 @@
         <v>0</v>
       </c>
       <c r="E40" t="n">
-        <v>9.9</v>
+        <v>1969</v>
       </c>
       <c r="F40" t="n">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>安徽·合肥·蜀山区</t>
+          <t>昆士兰·昆士兰</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>117.181802,31.865204</t>
+          <t>146.741207,-17.711625</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>香道温泉，带你体验“新中式”汤泉！</t>
+          <t>美丽的珊瑚群</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>1866486318</v>
+        <v>25603024</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>2019年深圳沙井兰花展</t>
+          <t>长江观音景区</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1952,34 +1952,34 @@
         <v>0</v>
       </c>
       <c r="E41" t="n">
-        <v>70</v>
+        <v>21.5</v>
       </c>
       <c r="F41" t="n">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>广东·深圳·宝安区</t>
+          <t>江苏·南京·栖霞区</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>113.865973,22.823594</t>
+          <t>118.803931,32.133416</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>满兰花的半截树桩吸引了目光</t>
+          <t>长江沿岸以观音文化为主题的景区</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>3132175194</v>
+        <v>1077114260</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>百花洲芙蓉馆</t>
+          <t>悉尼塔</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1988,33 +1988,37 @@
         </is>
       </c>
       <c r="D42" t="n">
-        <v>0</v>
+        <v>3.6</v>
       </c>
       <c r="E42" t="n">
-        <v>128</v>
+        <v>82.7</v>
       </c>
       <c r="F42" t="n">
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>山东·济南·历下区</t>
+          <t>新南威尔士州·悉尼</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>117.031835,36.677426</t>
-        </is>
-      </c>
-      <c r="I42" t="inlineStr"/>
+          <t>151.20876,-33.870451</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>金顶的悉尼塔(AMP Tower)建成于1981年，是世界伟达联邦的一员。楼高300米（展望台离地高250米），由56根</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>2935695043</v>
+        <v>4193588611</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>黑虎泉</t>
+          <t>南市食品街</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -2023,37 +2027,37 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>3.9</v>
+        <v>5</v>
       </c>
       <c r="E43" t="n">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="F43" t="n">
-        <v>2</v>
+        <v>70</v>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>山东·济南·历下区</t>
+          <t>天津·天津·和平区</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>117.039676,36.668445</t>
+          <t>117.191246,39.138647</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>石雕虎头泉水喷出，波澜汹汹，水声喧喧</t>
+          <t>有鲁迅描写的“咸亨酒店”</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>1011316032</v>
+        <v>2608360544</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>鹤冈八幡宫</t>
+          <t>悉尼杜莎夫人蜡像馆</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -2065,34 +2069,34 @@
         <v>0</v>
       </c>
       <c r="E44" t="n">
-        <v>308</v>
+        <v>110</v>
       </c>
       <c r="F44" t="n">
-        <v>69</v>
+        <v>4</v>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>神奈川县·镰仓</t>
+          <t>新南威尔士州·悉尼</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>139.556416666667,35.3261111111111</t>
+          <t>151.201508,-33.869791</t>
         </is>
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>祭祀八幡神的神社</t>
+          <t>看美丽栩栩如生的澳洲名模、皮特夫妇等</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>893606031</v>
+        <v>2829381737</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>天津滨海航母雪域王国</t>
+          <t>悉尼歌剧院</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -2101,76 +2105,76 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>0</v>
+        <v>3.7</v>
       </c>
       <c r="E45" t="n">
-        <v>660</v>
+        <v>96</v>
       </c>
       <c r="F45" t="n">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>天津·天津·天津泰达航母主题公园</t>
+          <t>新南威尔士州·悉尼</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>117.815038,39.162213</t>
+          <t>151.2152967,-33.8567844</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>泰达航母第四届“雪域王国”邀您开滑</t>
+          <t>悉尼歌剧院是20世纪世界七大奇迹之一</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>1192886682</v>
+        <v>2301889020</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>花水湾温泉旅游度假区</t>
+          <t>花水湾锦泰温泉</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>4A</t>
+          <t>无</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>3.5</v>
+        <v>0</v>
       </c>
       <c r="E46" t="n">
-        <v>47</v>
+        <v>79.90000000000001</v>
       </c>
       <c r="F46" t="n">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>四川·成都·大邑县</t>
+          <t>四川·成都·花水湾温泉旅游度假区</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>103.268238,30.569815</t>
+          <t>103.268273,30.57008</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>环境优美，休闲度假的好去处</t>
+          <t>花水湾温泉的特色——变色奇泉</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>2437128342</v>
+        <v>4263621879</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>海河公园</t>
+          <t>香道温泉会馆</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -2185,35 +2189,35 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>64</t>
+          <t>9.9</t>
         </is>
       </c>
       <c r="F47" t="n">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>天津·天津·和平区</t>
+          <t>安徽·合肥·蜀山区</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>117.218779,39.136942</t>
+          <t>117.181802,31.865204</t>
         </is>
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>海河公园、游玩、休憩的地方之一。在三岔口紧靠狮子林桥的水面上，有两组铜质塑像，这是海河公园的起点。其中，一组塑像是两条雄</t>
+          <t>香道温泉，带你体验“新中式”汤泉！</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>4152824504</v>
+        <v>1866486318</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>崇州国庆金秋田园灯会</t>
+          <t>2019年深圳沙井兰花展</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -2226,35 +2230,37 @@
           <t>0.0</t>
         </is>
       </c>
-      <c r="E48" t="n">
-        <v>0</v>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>70</t>
+        </is>
       </c>
       <c r="F48" t="n">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>四川·成都·崇州市</t>
+          <t>广东·深圳·宝安区</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>103.714815,30.712283</t>
+          <t>113.865973,22.823594</t>
         </is>
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>夜晚去田园花海，领略梦幻光影</t>
+          <t>满兰花的半截树桩吸引了目光</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>2983420679</v>
+        <v>3132175194</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>大堡礁</t>
+          <t>百花洲芙蓉馆</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -2269,35 +2275,31 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>1969</t>
+          <t>128</t>
         </is>
       </c>
       <c r="F49" t="n">
-        <v>86</v>
+        <v>47</v>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>昆士兰·昆士兰</t>
+          <t>山东·济南·历下区</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>146.741207,-17.711625</t>
-        </is>
-      </c>
-      <c r="I49" t="inlineStr">
-        <is>
-          <t>美丽的珊瑚群</t>
-        </is>
-      </c>
+          <t>117.031835,36.677426</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>1077114260</v>
+        <v>8602358</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>悉尼塔</t>
+          <t>解放阁</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -2307,40 +2309,40 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>3.6</t>
+          <t>3.7</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>82.7</t>
+          <t>109</t>
         </is>
       </c>
       <c r="F50" t="n">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>新南威尔士州·悉尼</t>
+          <t>山东·济南·历下区</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>151.20876,-33.870451</t>
+          <t>117.040064,36.668997</t>
         </is>
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>金顶的悉尼塔(AMP Tower)建成于1981年，是世界伟达联邦的一员。楼高300米（展望台离地高250米），由56根</t>
+          <t>纪念济南解放</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>4193588611</v>
+        <v>1975419947</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>南市食品街</t>
+          <t>济南芙蓉街</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -2350,40 +2352,40 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>5.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>50</t>
+          <t>100</t>
         </is>
       </c>
       <c r="F51" t="n">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>天津·天津·和平区</t>
+          <t>山东·济南·历下区</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>117.191246,39.138647</t>
+          <t>117.029527,36.675147</t>
         </is>
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>有鲁迅描写的“咸亨酒店”</t>
+          <t>流水潺潺，垂柳依依，意境优雅而享誉四海</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>2829381737</v>
+        <v>2828482046</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>悉尼歌剧院</t>
+          <t>邦迪海滩</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -2393,16 +2395,16 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>3.7</t>
+          <t>5.0</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>96</t>
+          <t>123</t>
         </is>
       </c>
       <c r="F52" t="n">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="G52" t="inlineStr">
         <is>
@@ -2411,22 +2413,22 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>151.2152967,-33.8567844</t>
+          <t>151.2766845,-33.8914755</t>
         </is>
       </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t>悉尼歌剧院是20世纪世界七大奇迹之一</t>
+          <t>日光浴和冲浪的绝佳地点</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>2301889020</v>
+        <v>1011316032</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>花水湾锦泰温泉</t>
+          <t>鹤冈八幡宫</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -2441,35 +2443,35 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>79.9</t>
+          <t>308</t>
         </is>
       </c>
       <c r="F53" t="n">
-        <v>94</v>
+        <v>77</v>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>四川·成都·花水湾温泉旅游度假区</t>
+          <t>神奈川县·镰仓</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>103.268273,30.57008</t>
+          <t>139.556416666667,35.3261111111111</t>
         </is>
       </c>
       <c r="I53" t="inlineStr">
         <is>
-          <t>花水湾温泉的特色——变色奇泉</t>
+          <t>祭祀八幡神的神社</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>8602358</v>
+        <v>893606031</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>解放阁</t>
+          <t>天津滨海航母雪域王国</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -2479,40 +2481,40 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>3.7</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>109</t>
+          <t>660</t>
         </is>
       </c>
       <c r="F54" t="n">
-        <v>75</v>
+        <v>95</v>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>山东·济南·历下区</t>
+          <t>天津·天津·天津泰达航母主题公园</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>117.040064,36.668997</t>
+          <t>117.815038,39.162213</t>
         </is>
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>纪念济南解放</t>
+          <t>泰达航母第四届“雪域王国”邀您开滑</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>1975419947</v>
+        <v>1908747770</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>济南芙蓉街</t>
+          <t>皇家植物园</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -2522,40 +2524,40 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>3.6</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>166</t>
         </is>
       </c>
       <c r="F55" t="n">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>山东·济南·历下区</t>
+          <t>维多利亚省·墨尔本</t>
         </is>
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>117.029527,36.675147</t>
+          <t>151.216569632292,-33.8641849762996</t>
         </is>
       </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t>流水潺潺，垂柳依依，意境优雅而享誉四海</t>
+          <t>一望无际的绿茵花园</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>2828482046</v>
+        <v>1587446860</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>邦迪海滩</t>
+          <t>悉尼海港大桥</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -2565,16 +2567,16 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>5.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>123</t>
+          <t>743</t>
         </is>
       </c>
       <c r="F56" t="n">
-        <v>84</v>
+        <v>62</v>
       </c>
       <c r="G56" t="inlineStr">
         <is>
@@ -2583,22 +2585,22 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>151.2766845,-33.8914755</t>
+          <t>151.2107871,-33.8523063</t>
         </is>
       </c>
       <c r="I56" t="inlineStr">
         <is>
-          <t>日光浴和冲浪的绝佳地点</t>
+          <t>一道横贯海湾的长虹，早期悉尼的代表建筑</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>1908747770</v>
+        <v>1626944140</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>皇家植物园</t>
+          <t>诺曼外堡礁</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -2608,40 +2610,40 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>3.6</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>166</t>
+          <t>726</t>
         </is>
       </c>
       <c r="F57" t="n">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>维多利亚省·墨尔本</t>
+          <t>昆士兰·大堡礁</t>
         </is>
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>151.216569632292,-33.8641849762996</t>
+          <t>147.699192181229,-18.2870671744257</t>
         </is>
       </c>
       <c r="I57" t="inlineStr">
         <is>
-          <t>一望无际的绿茵花园</t>
+          <t>论大人小孩都能找到适合的项目</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>1587446860</v>
+        <v>2462349966</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>悉尼海港大桥</t>
+          <t>悉尼海德公园</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -2651,16 +2653,16 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>3.6</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>743</t>
+          <t>1755</t>
         </is>
       </c>
       <c r="F58" t="n">
-        <v>87</v>
+        <v>43</v>
       </c>
       <c r="G58" t="inlineStr">
         <is>
@@ -2669,22 +2671,22 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>151.2107871,-33.8523063</t>
+          <t>151.211273193359,-33.8731368400047</t>
         </is>
       </c>
       <c r="I58" t="inlineStr">
         <is>
-          <t>一道横贯海湾的长虹，早期悉尼的代表建筑</t>
+          <t>历史悠久的城市公园</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>1626944140</v>
+        <v>4152824504</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>诺曼外堡礁</t>
+          <t>崇州国庆金秋田园灯会</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -2697,37 +2699,35 @@
           <t>0.0</t>
         </is>
       </c>
-      <c r="E59" t="inlineStr">
-        <is>
-          <t>726</t>
-        </is>
+      <c r="E59" t="n">
+        <v>0</v>
       </c>
       <c r="F59" t="n">
-        <v>95</v>
+        <v>0</v>
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>昆士兰·大堡礁</t>
+          <t>四川·成都·崇州市</t>
         </is>
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>147.699192181229,-18.2870671744257</t>
+          <t>103.714815,30.712283</t>
         </is>
       </c>
       <c r="I59" t="inlineStr">
         <is>
-          <t>论大人小孩都能找到适合的项目</t>
+          <t>夜晚去田园花海，领略梦幻光影</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>2462349966</v>
+        <v>2048431853</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>悉尼海德公园</t>
+          <t>玫瑰湾</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -2737,16 +2737,16 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>3.6</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>1755</t>
+          <t>166</t>
         </is>
       </c>
       <c r="F60" t="n">
-        <v>81</v>
+        <v>31</v>
       </c>
       <c r="G60" t="inlineStr">
         <is>
@@ -2755,22 +2755,22 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>151.211273193359,-33.8731368400047</t>
+          <t>151.266460478306,-33.8732733633383</t>
         </is>
       </c>
       <c r="I60" t="inlineStr">
         <is>
-          <t>历史悠久的城市公园</t>
+          <t>玫瑰湾是悉尼举行各种各样展览。湾内棕榈婆娑，绿草茵茵，游戏场内儿童嬉戏，露天咖啡厅人们休憩谈天，港内有许多处水池及喷泉，</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>2048431853</v>
+        <v>3441455959</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>玫瑰湾</t>
+          <t>悉尼鱼市场</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -2785,11 +2785,11 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>166</t>
+          <t>451</t>
         </is>
       </c>
       <c r="F61" t="n">
-        <v>41</v>
+        <v>76</v>
       </c>
       <c r="G61" t="inlineStr">
         <is>
@@ -2798,12 +2798,12 @@
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>151.266460478306,-33.8732733633383</t>
+          <t>151.1925959,-33.873102</t>
         </is>
       </c>
       <c r="I61" t="inlineStr">
         <is>
-          <t>玫瑰湾是悉尼举行各种各样展览。湾内棕榈婆娑，绿草茵茵，游戏场内儿童嬉戏，露天咖啡厅人们休憩谈天，港内有许多处水池及喷泉，</t>
+          <t>参加鱼市幕后之旅，一览鱼市背后的秘密</t>
         </is>
       </c>
     </row>

</xml_diff>